<commit_message>
Rollback THIN Route 1 implementation - violated framework agnosticism
- Restored orchestrator.py to original state (removed framework-aware enhancements)
- Restored thin_litellm_client.py to original state (removed safety checks)
- Deleted framework_loader.py (contained framework-specific assumptions)
- Deleted orchestrator_enhancement.py (contained CFF-specific patterns)
- Deleted frameworks/cohesive_flourishing_framework_v2.yaml (hardcoded structure)
- Added SESSION_ROLLBACK_HANDOFF.md documenting what was achieved and why it was rolled back

Core issue: Solution successfully eliminated process hallucination but violated THIN principles by embedding framework/corpus-specific assumptions into software rather than keeping it generic.

Problem remains: Need truly framework-agnostic solution that works with any framework, content type, and output format while maintaining THIN architecture.


Former-commit-id: 5665191886e3bac3a3d208c85513643a369e02b4
</commit_message>
<xml_diff>
--- a/projects/vanderveen/combined-data-set-xlsx.xlsx
+++ b/projects/vanderveen/combined-data-set-xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mckinneyvoss/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/discernus/projects/vanderveen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A05A4A19-6E6F-4B27-8736-2A719FA4E586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675253A0-BB44-5F4A-858F-207F23DA4003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="36280" windowHeight="29860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -314,11 +314,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -438,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -466,7 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -475,10 +477,6 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -486,15 +484,12 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -504,12 +499,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -519,84 +508,67 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -882,16 +854,16 @@
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="48">
-      <c r="A1" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="55"/>
+    <row r="1" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -938,7 +910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -989,7 +961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1009,7 +981,7 @@
       <c r="G3" s="7">
         <v>1</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="6">
@@ -1024,17 +996,17 @@
       <c r="L3" s="7">
         <v>0.2</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="17" t="s">
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
@@ -1071,21 +1043,21 @@
       <c r="N4" s="12">
         <v>0</v>
       </c>
-      <c r="O4" s="18">
-        <v>0</v>
-      </c>
-      <c r="P4" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="17" t="s">
+      <c r="O4" s="16">
+        <v>0</v>
+      </c>
+      <c r="P4" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="17"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1116,18 +1088,18 @@
       <c r="L5" s="10">
         <v>0.3</v>
       </c>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="17" t="s">
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="6">
@@ -1157,17 +1129,17 @@
       <c r="L6" s="10">
         <v>1</v>
       </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="17" t="s">
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
@@ -1192,17 +1164,17 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="17" t="s">
+      <c r="M7" s="14"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="5" t="s">
         <v>23</v>
       </c>
@@ -1233,17 +1205,17 @@
       <c r="L8" s="7">
         <v>0</v>
       </c>
-      <c r="M8" s="15"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="17" t="s">
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="17"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
@@ -1274,17 +1246,17 @@
       <c r="L9" s="10">
         <v>0.6</v>
       </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="17" t="s">
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
@@ -1300,22 +1272,22 @@
       <c r="G10" s="7">
         <v>0.1</v>
       </c>
-      <c r="H10" s="20"/>
+      <c r="H10" s="18"/>
       <c r="I10" s="6"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="17" t="s">
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
@@ -1346,17 +1318,17 @@
       <c r="L11" s="7">
         <v>1.3</v>
       </c>
-      <c r="M11" s="15"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="17" t="s">
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1387,17 +1359,17 @@
       <c r="L12" s="7">
         <v>2</v>
       </c>
-      <c r="M12" s="15"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="17" t="s">
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="5" t="s">
         <v>31</v>
       </c>
@@ -1428,17 +1400,17 @@
       <c r="L13" s="7">
         <v>1.3</v>
       </c>
-      <c r="M13" s="15"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="17" t="s">
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="17"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
@@ -1469,17 +1441,17 @@
       <c r="L14" s="7">
         <v>1.8</v>
       </c>
-      <c r="M14" s="15"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="17" t="s">
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="17"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="5" t="s">
         <v>9</v>
       </c>
@@ -1510,17 +1482,17 @@
       <c r="L15" s="7">
         <v>1.8</v>
       </c>
-      <c r="M15" s="15"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="17" t="s">
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="5" t="s">
         <v>9</v>
       </c>
@@ -1551,23 +1523,23 @@
       <c r="L16" s="10">
         <v>1.5</v>
       </c>
-      <c r="M16" s="21" t="s">
+      <c r="M16" s="11" t="s">
         <v>16</v>
       </c>
       <c r="N16" s="12">
         <v>1</v>
       </c>
-      <c r="O16" s="18">
-        <v>1</v>
-      </c>
-      <c r="P16" s="18">
+      <c r="O16" s="16">
+        <v>1</v>
+      </c>
+      <c r="P16" s="16">
         <v>2</v>
       </c>
-      <c r="Q16" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="Q16" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -1587,28 +1559,28 @@
       <c r="G17" s="7">
         <v>1</v>
       </c>
-      <c r="H17" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="23">
+      <c r="H17" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="20">
         <v>0.3</v>
       </c>
-      <c r="J17" s="24">
+      <c r="J17" s="21">
         <v>0.8</v>
       </c>
-      <c r="K17" s="24">
-        <v>0.2</v>
-      </c>
-      <c r="L17" s="24">
+      <c r="K17" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="L17" s="21">
         <v>0.6</v>
       </c>
-      <c r="M17" s="15"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
@@ -1616,16 +1588,16 @@
       <c r="C18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="6">
         <v>0.9</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="7">
         <v>0.9</v>
       </c>
-      <c r="F18" s="26">
-        <v>1.5</v>
-      </c>
-      <c r="G18" s="26">
+      <c r="F18" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="G18" s="7">
         <v>0.8</v>
       </c>
       <c r="H18" s="8" t="s">
@@ -1643,13 +1615,13 @@
       <c r="L18" s="10">
         <v>1</v>
       </c>
-      <c r="M18" s="15"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
@@ -1684,17 +1656,17 @@
       <c r="L19" s="7">
         <v>2</v>
       </c>
-      <c r="M19" s="15"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="27" t="s">
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="27"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="5" t="s">
         <v>9</v>
       </c>
@@ -1725,18 +1697,18 @@
       <c r="L20" s="10">
         <v>0.6</v>
       </c>
-      <c r="M20" s="15"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="28" t="s">
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29" t="s">
+      <c r="B21" s="23"/>
+      <c r="C21" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="9">
@@ -1767,12 +1739,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="30" t="s">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="29" t="s">
+      <c r="B22" s="23"/>
+      <c r="C22" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="9">
@@ -1803,12 +1775,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="30" t="s">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="29" t="s">
+      <c r="B23" s="23"/>
+      <c r="C23" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="9">
@@ -1839,12 +1811,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="30" t="s">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="29" t="s">
+      <c r="B24" s="23"/>
+      <c r="C24" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="9">
@@ -1875,12 +1847,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="29" t="s">
+      <c r="B25" s="23"/>
+      <c r="C25" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="9">
@@ -1911,12 +1883,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="30" t="s">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="29" t="s">
+      <c r="B26" s="23"/>
+      <c r="C26" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="9">
@@ -1947,12 +1919,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="31" t="s">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="29" t="s">
+      <c r="B27" s="26"/>
+      <c r="C27" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="9">
@@ -1983,12 +1955,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
-      <c r="A28" s="30" t="s">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="29" t="s">
+      <c r="B28" s="23"/>
+      <c r="C28" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="9">
@@ -2019,12 +1991,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
-      <c r="A29" s="30" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="29" t="s">
+      <c r="B29" s="23"/>
+      <c r="C29" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="9">
@@ -2049,12 +2021,12 @@
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
     </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="30" t="s">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="29" t="s">
+      <c r="B30" s="23"/>
+      <c r="C30" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="9">
@@ -2079,12 +2051,12 @@
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
     </row>
-    <row r="31" spans="1:17" ht="48">
-      <c r="A31" s="33" t="s">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="29" t="s">
+      <c r="B31" s="27"/>
+      <c r="C31" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="9">
@@ -2115,12 +2087,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
-      <c r="A32" s="35" t="s">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="29" t="s">
+      <c r="B32" s="26"/>
+      <c r="C32" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="9">
@@ -2151,12 +2123,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="28" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="29" t="s">
+      <c r="B33" s="23"/>
+      <c r="C33" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="9">
@@ -2187,12 +2159,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="35" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="36"/>
-      <c r="C34" s="29" t="s">
+      <c r="B34" s="26"/>
+      <c r="C34" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="9">
@@ -2223,12 +2195,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="30" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="29" t="s">
+      <c r="B35" s="23"/>
+      <c r="C35" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="9">
@@ -2246,7 +2218,7 @@
       <c r="H35" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I35" s="37">
+      <c r="I35" s="9">
         <v>0.8</v>
       </c>
       <c r="J35" s="10">
@@ -2259,12 +2231,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="38" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="29" t="s">
+      <c r="B36" s="29"/>
+      <c r="C36" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="9">
@@ -2295,12 +2267,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="40" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="29" t="s">
+      <c r="B37" s="31"/>
+      <c r="C37" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="9">
@@ -2331,12 +2303,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="42" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="29" t="s">
+      <c r="B38" s="33"/>
+      <c r="C38" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="9">
@@ -2367,12 +2339,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="40" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="29" t="s">
+      <c r="B39" s="31"/>
+      <c r="C39" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="9">
@@ -2403,12 +2375,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="40" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="41"/>
-      <c r="C40" s="29" t="s">
+      <c r="B40" s="31"/>
+      <c r="C40" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="6">
@@ -2439,12 +2411,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="40" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="41"/>
-      <c r="C41" s="29" t="s">
+      <c r="B41" s="31"/>
+      <c r="C41" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="6">
@@ -2475,12 +2447,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="40" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="29" t="s">
+      <c r="B42" s="31"/>
+      <c r="C42" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="6">
@@ -2511,12 +2483,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="56" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="57"/>
-      <c r="C43" s="29" t="s">
+      <c r="B43" s="44"/>
+      <c r="C43" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="9">
@@ -2547,12 +2519,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="56" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="57"/>
-      <c r="C44" s="29" t="s">
+      <c r="B44" s="44"/>
+      <c r="C44" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="9">
@@ -2583,12 +2555,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="16" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="29" t="s">
+      <c r="B45" s="14"/>
+      <c r="C45" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D45" s="9">
@@ -2619,12 +2591,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
-      <c r="A46" s="16" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="29" t="s">
+      <c r="B46" s="14"/>
+      <c r="C46" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="9">
@@ -2655,12 +2627,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="15" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="29" t="s">
+      <c r="B47" s="14"/>
+      <c r="C47" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="9">
@@ -2691,12 +2663,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="58" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="59"/>
-      <c r="C48" s="29" t="s">
+      <c r="B48" s="46"/>
+      <c r="C48" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="9">
@@ -2727,12 +2699,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
-      <c r="A49" s="15" t="s">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="16"/>
-      <c r="C49" s="29" t="s">
+      <c r="B49" s="14"/>
+      <c r="C49" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D49" s="9">
@@ -2763,12 +2735,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
-      <c r="A50" s="15" t="s">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="29" t="s">
+      <c r="B50" s="14"/>
+      <c r="C50" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="9">
@@ -2799,12 +2771,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
-      <c r="A51" s="15" t="s">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="29" t="s">
+      <c r="B51" s="14"/>
+      <c r="C51" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="9">
@@ -2835,12 +2807,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
-      <c r="A52" s="44" t="s">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B52" s="45"/>
-      <c r="C52" s="29" t="s">
+      <c r="B52" s="17"/>
+      <c r="C52" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D52" s="9">
@@ -2861,22 +2833,22 @@
       <c r="I52" s="9">
         <v>0.1</v>
       </c>
-      <c r="J52" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="K52" s="45">
-        <v>0</v>
-      </c>
-      <c r="L52" s="45">
+      <c r="J52" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="K52" s="17">
+        <v>0</v>
+      </c>
+      <c r="L52" s="17">
         <v>0.8</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
-      <c r="A53" s="56" t="s">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="57"/>
-      <c r="C53" s="29" t="s">
+      <c r="B53" s="44"/>
+      <c r="C53" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D53" s="9">
@@ -2897,34 +2869,34 @@
       <c r="I53" s="9">
         <v>1.7</v>
       </c>
-      <c r="J53" s="19">
+      <c r="J53" s="17">
         <v>2</v>
       </c>
-      <c r="K53" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="L53" s="19">
+      <c r="K53" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L53" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
-      <c r="A54" s="56" t="s">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B54" s="57"/>
-      <c r="C54" s="29" t="s">
+      <c r="B54" s="44"/>
+      <c r="C54" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D54" s="9">
         <v>1.2</v>
       </c>
-      <c r="E54" s="19">
-        <v>1</v>
-      </c>
-      <c r="F54" s="19">
-        <v>1</v>
-      </c>
-      <c r="G54" s="19">
+      <c r="E54" s="17">
+        <v>1</v>
+      </c>
+      <c r="F54" s="17">
+        <v>1</v>
+      </c>
+      <c r="G54" s="17">
         <v>1.8</v>
       </c>
       <c r="H54" s="8" t="s">
@@ -2933,34 +2905,34 @@
       <c r="I54" s="9">
         <v>1.3</v>
       </c>
-      <c r="J54" s="19">
+      <c r="J54" s="17">
         <v>1.3</v>
       </c>
-      <c r="K54" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="L54" s="19">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14">
-      <c r="A55" s="46" t="s">
+      <c r="K54" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L54" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B55" s="15"/>
-      <c r="C55" s="29" t="s">
+      <c r="B55" s="14"/>
+      <c r="C55" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D55" s="9">
         <v>0.4</v>
       </c>
-      <c r="E55" s="19">
+      <c r="E55" s="17">
         <v>0.3</v>
       </c>
-      <c r="F55" s="19">
+      <c r="F55" s="17">
         <v>0.4</v>
       </c>
-      <c r="G55" s="19">
+      <c r="G55" s="17">
         <v>0.3</v>
       </c>
       <c r="H55" s="8" t="s">
@@ -2969,34 +2941,34 @@
       <c r="I55" s="9">
         <v>0.2</v>
       </c>
-      <c r="J55" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="K55" s="19">
-        <v>0</v>
-      </c>
-      <c r="L55" s="19">
+      <c r="J55" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="K55" s="17">
+        <v>0</v>
+      </c>
+      <c r="L55" s="17">
         <v>0.3</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
-      <c r="A56" s="47" t="s">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="15"/>
-      <c r="C56" s="29" t="s">
+      <c r="B56" s="14"/>
+      <c r="C56" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="9">
         <v>1.2</v>
       </c>
-      <c r="E56" s="19">
+      <c r="E56" s="17">
         <v>0.9</v>
       </c>
-      <c r="F56" s="19">
+      <c r="F56" s="17">
         <v>0.9</v>
       </c>
-      <c r="G56" s="19">
+      <c r="G56" s="17">
         <v>1.5</v>
       </c>
       <c r="H56" s="8" t="s">
@@ -3005,34 +2977,34 @@
       <c r="I56" s="9">
         <v>1.4</v>
       </c>
-      <c r="J56" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="K56" s="19">
+      <c r="J56" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="K56" s="17">
         <v>1.3</v>
       </c>
-      <c r="L56" s="19">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
-      <c r="A57" s="47" t="s">
+      <c r="L56" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="B57" s="15"/>
-      <c r="C57" s="29" t="s">
+      <c r="B57" s="14"/>
+      <c r="C57" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="9">
         <v>0.1</v>
       </c>
-      <c r="E57" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="F57" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="G57" s="19">
+      <c r="E57" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="F57" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="G57" s="17">
         <v>0.3</v>
       </c>
       <c r="H57" s="8" t="s">
@@ -3041,34 +3013,34 @@
       <c r="I57" s="9">
         <v>0.1</v>
       </c>
-      <c r="J57" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="K57" s="19">
-        <v>0</v>
-      </c>
-      <c r="L57" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
-      <c r="A58" s="47" t="s">
+      <c r="J57" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="K57" s="17">
+        <v>0</v>
+      </c>
+      <c r="L57" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="B58" s="15"/>
-      <c r="C58" s="29" t="s">
+      <c r="B58" s="14"/>
+      <c r="C58" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="9">
         <v>0.1</v>
       </c>
-      <c r="E58" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="F58" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="G58" s="19">
+      <c r="E58" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="F58" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="G58" s="17">
         <v>0</v>
       </c>
       <c r="H58" s="8" t="s">
@@ -3077,36 +3049,34 @@
       <c r="I58" s="9">
         <v>0.1</v>
       </c>
-      <c r="J58" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="K58" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="L58" s="19">
-        <v>0</v>
-      </c>
-      <c r="M58" s="48"/>
-      <c r="N58" s="48"/>
-    </row>
-    <row r="59" spans="1:14">
-      <c r="A59" s="47" t="s">
+      <c r="J58" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="K58" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L58" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B59" s="15"/>
-      <c r="C59" s="29" t="s">
+      <c r="B59" s="14"/>
+      <c r="C59" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="9">
         <v>1.2</v>
       </c>
-      <c r="E59" s="19">
+      <c r="E59" s="17">
         <v>1.3</v>
       </c>
-      <c r="F59" s="19">
+      <c r="F59" s="17">
         <v>1.3</v>
       </c>
-      <c r="G59" s="19">
+      <c r="G59" s="17">
         <v>1.5</v>
       </c>
       <c r="H59" s="8" t="s">
@@ -3115,36 +3085,34 @@
       <c r="I59" s="9">
         <v>1.3</v>
       </c>
-      <c r="J59" s="19">
-        <v>0</v>
-      </c>
-      <c r="K59" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="L59" s="19">
-        <v>0</v>
-      </c>
-      <c r="M59" s="48"/>
-      <c r="N59" s="48"/>
-    </row>
-    <row r="60" spans="1:14">
-      <c r="A60" s="15" t="s">
+      <c r="J59" s="17">
+        <v>0</v>
+      </c>
+      <c r="K59" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L59" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="15"/>
-      <c r="C60" s="29" t="s">
+      <c r="B60" s="14"/>
+      <c r="C60" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D60" s="9">
         <v>0.2</v>
       </c>
-      <c r="E60" s="19">
-        <v>0</v>
-      </c>
-      <c r="F60" s="19">
+      <c r="E60" s="17">
+        <v>0</v>
+      </c>
+      <c r="F60" s="17">
         <v>0.4</v>
       </c>
-      <c r="G60" s="19">
+      <c r="G60" s="17">
         <v>0.1</v>
       </c>
       <c r="H60" s="8" t="s">
@@ -3153,36 +3121,34 @@
       <c r="I60" s="9">
         <v>0.4</v>
       </c>
-      <c r="J60" s="19">
-        <v>0</v>
-      </c>
-      <c r="K60" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="L60" s="19">
-        <v>0</v>
-      </c>
-      <c r="M60" s="49"/>
-      <c r="N60" s="48"/>
-    </row>
-    <row r="61" spans="1:14">
-      <c r="A61" s="50" t="s">
+      <c r="J60" s="17">
+        <v>0</v>
+      </c>
+      <c r="K60" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L60" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B61" s="50"/>
-      <c r="C61" s="29" t="s">
+      <c r="B61" s="37"/>
+      <c r="C61" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D61" s="9">
         <v>0.1</v>
       </c>
-      <c r="E61" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="F61" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="G61" s="19">
+      <c r="E61" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="F61" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="G61" s="17">
         <v>0</v>
       </c>
       <c r="H61" s="8" t="s">
@@ -3191,117 +3157,105 @@
       <c r="I61" s="9">
         <v>0</v>
       </c>
-      <c r="J61" s="19">
-        <v>0</v>
-      </c>
-      <c r="K61" s="19">
-        <v>0</v>
-      </c>
-      <c r="L61" s="19">
-        <v>0</v>
-      </c>
-      <c r="M61" s="49"/>
-      <c r="N61" s="48"/>
-    </row>
-    <row r="62" spans="1:14">
-      <c r="A62" s="54"/>
-      <c r="B62" s="54"/>
-      <c r="C62" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D62" s="51"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="53"/>
+      <c r="J61" s="17">
+        <v>0</v>
+      </c>
+      <c r="K61" s="17">
+        <v>0</v>
+      </c>
+      <c r="L61" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62" s="41"/>
+      <c r="B62" s="41"/>
+      <c r="C62" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="38"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="40"/>
       <c r="H62" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I62" s="51"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="52"/>
-      <c r="L62" s="53"/>
-      <c r="M62" s="49"/>
-      <c r="N62" s="48"/>
-    </row>
-    <row r="63" spans="1:14">
-      <c r="A63" s="15"/>
-      <c r="B63" s="15"/>
-      <c r="C63" s="29" t="s">
+      <c r="I62" s="38"/>
+      <c r="J62" s="39"/>
+      <c r="K62" s="39"/>
+      <c r="L62" s="40"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D63" s="9"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
       <c r="H63" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I63" s="9"/>
-      <c r="J63" s="19"/>
-      <c r="K63" s="19"/>
-      <c r="L63" s="19"/>
-      <c r="M63" s="49"/>
-      <c r="N63" s="48"/>
-    </row>
-    <row r="64" spans="1:14">
-      <c r="A64" s="15"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="29" t="s">
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D64" s="9"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="19"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
       <c r="H64" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I64" s="9"/>
-      <c r="J64" s="19"/>
-      <c r="K64" s="19"/>
-      <c r="L64" s="19"/>
-      <c r="M64" s="48"/>
-      <c r="N64" s="48"/>
-    </row>
-    <row r="65" spans="1:14">
-      <c r="A65" s="15"/>
-      <c r="B65" s="15"/>
-      <c r="C65" s="29" t="s">
+      <c r="J64" s="17"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D65" s="9"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="17"/>
       <c r="H65" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I65" s="9"/>
-      <c r="J65" s="19"/>
-      <c r="K65" s="19"/>
-      <c r="L65" s="19"/>
-      <c r="M65" s="48"/>
-      <c r="N65" s="48"/>
-    </row>
-    <row r="66" spans="1:14">
-      <c r="A66" s="15"/>
-      <c r="B66" s="15"/>
-      <c r="C66" s="29" t="s">
+      <c r="J65" s="17"/>
+      <c r="K65" s="17"/>
+      <c r="L65" s="17"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D66" s="9"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
       <c r="H66" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I66" s="9"/>
-      <c r="J66" s="19"/>
-      <c r="K66" s="19"/>
-      <c r="L66" s="19"/>
-      <c r="M66" s="48"/>
-      <c r="N66" s="48"/>
+      <c r="J66" s="17"/>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>